<commit_message>
issue from american  add company name...
</commit_message>
<xml_diff>
--- a/doc/WeldFileFormat.xlsx
+++ b/doc/WeldFileFormat.xlsx
@@ -48,9 +48,6 @@
     <t xml:space="preserve">     Xa00 As String * &amp;HA</t>
   </si>
   <si>
-    <t xml:space="preserve">     Xa14 As String * &amp;HD</t>
-  </si>
-  <si>
     <t xml:space="preserve">     Xc10 As String * &amp;H4</t>
   </si>
   <si>
@@ -335,6 +332,10 @@
   </si>
   <si>
     <t xml:space="preserve">     H6(&amp;H1E - 1) As Byte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Xa14 As String * &amp;H6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -687,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -704,7 +705,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -727,7 +728,7 @@
         <v>0001</v>
       </c>
       <c r="G2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -750,7 +751,7 @@
         <v>0002</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -773,7 +774,7 @@
         <v>0003</v>
       </c>
       <c r="G4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -796,7 +797,7 @@
         <v>0004</v>
       </c>
       <c r="G5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -819,7 +820,7 @@
         <v>0008</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -842,7 +843,7 @@
         <v>0009</v>
       </c>
       <c r="G7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -865,15 +866,15 @@
         <v>000A</v>
       </c>
       <c r="G8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
@@ -888,12 +889,12 @@
         <v>002A</v>
       </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="B10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
@@ -908,7 +909,7 @@
         <v>002A</v>
       </c>
       <c r="G10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -931,15 +932,15 @@
         <v>002A</v>
       </c>
       <c r="G11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
@@ -954,7 +955,7 @@
         <v>0900</v>
       </c>
       <c r="G12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -974,7 +975,7 @@
         <v>0900</v>
       </c>
       <c r="G13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -994,7 +995,7 @@
         <v>0900</v>
       </c>
       <c r="G14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1002,7 +1003,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
@@ -1017,15 +1018,15 @@
         <v>090A</v>
       </c>
       <c r="G15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
@@ -1040,15 +1041,15 @@
         <v>0924</v>
       </c>
       <c r="G16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
@@ -1063,7 +1064,7 @@
         <v>0930</v>
       </c>
       <c r="G17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1083,15 +1084,15 @@
         <v>0930</v>
       </c>
       <c r="G18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
@@ -1106,7 +1107,7 @@
         <v>0A00</v>
       </c>
       <c r="G19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1126,7 +1127,7 @@
         <v>0A00</v>
       </c>
       <c r="G20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1134,7 +1135,7 @@
         <v>9</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
@@ -1149,15 +1150,15 @@
         <v>0A0A</v>
       </c>
       <c r="G21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
@@ -1172,15 +1173,15 @@
         <v>0A1A</v>
       </c>
       <c r="G22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
@@ -1195,7 +1196,7 @@
         <v>0A20</v>
       </c>
       <c r="G23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="12.75" customHeight="1">
@@ -1215,15 +1216,15 @@
         <v>0A20</v>
       </c>
       <c r="G24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
@@ -1238,7 +1239,7 @@
         <v>0C10</v>
       </c>
       <c r="G25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1255,7 +1256,7 @@
         <v>0C10</v>
       </c>
       <c r="G26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1275,15 +1276,15 @@
         <v>0C10</v>
       </c>
       <c r="G27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28">
         <f t="shared" si="0"/>
@@ -1298,25 +1299,25 @@
         <v>0C14</v>
       </c>
       <c r="G28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C33">
         <f t="shared" si="0"/>
@@ -1331,15 +1332,15 @@
         <v>0C19</v>
       </c>
       <c r="G33" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C34">
         <f t="shared" si="0"/>
@@ -1354,15 +1355,15 @@
         <v>0C1A</v>
       </c>
       <c r="G34" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C35">
         <f t="shared" si="0"/>
@@ -1377,15 +1378,22 @@
         <v>0C25</v>
       </c>
       <c r="G35" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+        <v>59</v>
+      </c>
+      <c r="I35">
+        <v>3092</v>
+      </c>
+      <c r="J35" t="str">
+        <f>DEC2HEX(I35,6)</f>
+        <v>000C14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C36">
         <f t="shared" si="0"/>
@@ -1400,10 +1408,14 @@
         <v>0C30</v>
       </c>
       <c r="G36" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+        <v>60</v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" ref="J36:J38" si="2">DEC2HEX(I36,6)</f>
+        <v>000000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -1420,15 +1432,19 @@
         <v>0C30</v>
       </c>
       <c r="G37" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+        <v>60</v>
+      </c>
+      <c r="J37" t="str">
+        <f t="shared" si="2"/>
+        <v>000000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C38">
         <f t="shared" si="0"/>
@@ -1443,10 +1459,14 @@
         <v>0D10</v>
       </c>
       <c r="G38" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+        <v>61</v>
+      </c>
+      <c r="J38" t="str">
+        <f t="shared" si="2"/>
+        <v>000000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1463,10 +1483,10 @@
         <v>0D10</v>
       </c>
       <c r="G39" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -1483,15 +1503,15 @@
         <v>0D10</v>
       </c>
       <c r="G40" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C41">
         <f t="shared" si="0"/>
@@ -1506,15 +1526,15 @@
         <v>0D1A</v>
       </c>
       <c r="G41" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C42">
         <f t="shared" si="0"/>
@@ -1529,15 +1549,15 @@
         <v>0D22</v>
       </c>
       <c r="G42" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C43">
         <f t="shared" si="0"/>
@@ -1552,10 +1572,10 @@
         <v>0D30</v>
       </c>
       <c r="G43" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -1572,18 +1592,18 @@
         <v>0D30</v>
       </c>
       <c r="G44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H44">
         <v>1410</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C45">
         <f t="shared" si="0"/>
@@ -1598,18 +1618,18 @@
         <v>0E1C</v>
       </c>
       <c r="G45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H45" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C46">
         <f t="shared" si="0"/>
@@ -1624,15 +1644,15 @@
         <v>0E1E</v>
       </c>
       <c r="G46" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C47">
         <f t="shared" si="0"/>
@@ -1647,15 +1667,15 @@
         <v>0E20</v>
       </c>
       <c r="G47" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C48">
         <f t="shared" si="0"/>
@@ -1670,15 +1690,15 @@
         <v>1410</v>
       </c>
       <c r="G48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C50">
         <f t="shared" si="0"/>
@@ -1693,15 +1713,15 @@
         <v>141C</v>
       </c>
       <c r="G50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C51">
         <f t="shared" si="0"/>
@@ -1716,15 +1736,15 @@
         <v>1423</v>
       </c>
       <c r="G51" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C52">
         <f t="shared" si="0"/>
@@ -1739,15 +1759,15 @@
         <v>1430</v>
       </c>
       <c r="G52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C54">
         <f t="shared" si="0"/>
@@ -1762,15 +1782,15 @@
         <v>144E</v>
       </c>
       <c r="G54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C55">
         <f t="shared" si="0"/>
@@ -1785,7 +1805,7 @@
         <v>144E</v>
       </c>
       <c r="G55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -1802,7 +1822,7 @@
         <v>144E</v>
       </c>
       <c r="G56" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -1819,7 +1839,7 @@
         <v>144E</v>
       </c>
       <c r="G57" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -1836,7 +1856,7 @@
         <v>144E</v>
       </c>
       <c r="G58" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -1853,7 +1873,7 @@
         <v>144E</v>
       </c>
       <c r="G59" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -1870,7 +1890,7 @@
         <v>144E</v>
       </c>
       <c r="G60" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>